<commit_message>
Corregido número de parte de conector B-C en PCB_C
</commit_message>
<xml_diff>
--- a/Hardware/Satelite/PCB_C/BOM_C.xlsx
+++ b/Hardware/Satelite/PCB_C/BOM_C.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21629"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\msys32\home\tmax4\esp\Hardware\Satelite\PCB_C\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3D6EAAF-7EA2-421F-86D0-F21F1A1492D0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B8BDB1-8BE1-4EA7-B455-6113DA63233D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="13320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PCB_C" sheetId="1" r:id="rId1"/>
@@ -115,9 +115,6 @@
     <t>AXTEC:Conector_PCB_B-C_Lado_C</t>
   </si>
   <si>
-    <t>53353-1071</t>
-  </si>
-  <si>
     <t>J4</t>
   </si>
   <si>
@@ -263,6 +260,9 @@
   </si>
   <si>
     <t>U1, U4</t>
+  </si>
+  <si>
+    <t>53353-2071</t>
   </si>
 </sst>
 </file>
@@ -750,48 +750,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="42">
-    <cellStyle name="20% - Énfasis1" xfId="19" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis2" xfId="23" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis3" xfId="27" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis4" xfId="31" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis5" xfId="35" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20% - Énfasis6" xfId="39" builtinId="50" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis1" xfId="20" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis2" xfId="24" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis3" xfId="28" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis4" xfId="32" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis5" xfId="36" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40% - Énfasis6" xfId="40" builtinId="51" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis1" xfId="21" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis2" xfId="25" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis3" xfId="29" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis4" xfId="33" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis5" xfId="37" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60% - Énfasis6" xfId="41" builtinId="52" customBuiltin="1"/>
-    <cellStyle name="Bueno" xfId="6" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Cálculo" xfId="11" builtinId="22" customBuiltin="1"/>
-    <cellStyle name="Celda de comprobación" xfId="13" builtinId="23" customBuiltin="1"/>
-    <cellStyle name="Celda vinculada" xfId="12" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Encabezado 1" xfId="2" builtinId="16" customBuiltin="1"/>
-    <cellStyle name="Encabezado 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Énfasis1" xfId="18" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Énfasis2" xfId="22" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Énfasis3" xfId="26" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Énfasis4" xfId="30" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Énfasis5" xfId="34" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Énfasis6" xfId="38" builtinId="49" customBuiltin="1"/>
-    <cellStyle name="Entrada" xfId="9" builtinId="20" customBuiltin="1"/>
-    <cellStyle name="Incorrecto" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Bad" xfId="7" builtinId="27" customBuiltin="1"/>
+    <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Notas" xfId="15" builtinId="10" customBuiltin="1"/>
-    <cellStyle name="Salida" xfId="10" builtinId="21" customBuiltin="1"/>
-    <cellStyle name="Texto de advertencia" xfId="14" builtinId="11" customBuiltin="1"/>
-    <cellStyle name="Texto explicativo" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Título" xfId="1" builtinId="15" customBuiltin="1"/>
-    <cellStyle name="Título 2" xfId="3" builtinId="17" customBuiltin="1"/>
-    <cellStyle name="Título 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -821,7 +821,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1121,18 +1121,18 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C23" sqref="C23"/>
+      <selection pane="bottomLeft" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.07421875" defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="2" max="2" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="35.3828125" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="68.7109375" customWidth="1"/>
-    <col min="5" max="5" width="26.85546875" customWidth="1"/>
+    <col min="4" max="4" width="68.69140625" customWidth="1"/>
+    <col min="5" max="5" width="26.84375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1149,12 +1149,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -1166,12 +1166,12 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>9</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
         <v>8</v>
@@ -1183,12 +1183,12 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
         <v>10</v>
@@ -1200,7 +1200,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1217,12 +1217,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>2</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C6" t="s">
         <v>16</v>
@@ -1234,7 +1234,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1251,7 +1251,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1268,7 +1268,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1299,225 +1299,225 @@
         <v>30</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>4</v>
       </c>
       <c r="B11" t="s">
+        <v>31</v>
+      </c>
+      <c r="C11" t="s">
         <v>32</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>33</v>
       </c>
-      <c r="D11" t="s">
+      <c r="E11" t="s">
         <v>34</v>
       </c>
-      <c r="E11" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>1</v>
       </c>
       <c r="B12" t="s">
+        <v>35</v>
+      </c>
+      <c r="C12" t="s">
         <v>36</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>37</v>
       </c>
-      <c r="D12" t="s">
+      <c r="E12" t="s">
         <v>38</v>
       </c>
-      <c r="E12" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>3</v>
       </c>
       <c r="B13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C13" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" t="s">
         <v>40</v>
       </c>
-      <c r="D13" t="s">
+      <c r="E13" t="s">
         <v>41</v>
       </c>
-      <c r="E13" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>44</v>
       </c>
-      <c r="D14" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C15" t="s">
+        <v>45</v>
+      </c>
+      <c r="D15" t="s">
         <v>46</v>
       </c>
-      <c r="D15" t="s">
+      <c r="E15" t="s">
         <v>47</v>
       </c>
-      <c r="E15" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>2</v>
       </c>
       <c r="B16" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C16" t="s">
+        <v>48</v>
+      </c>
+      <c r="D16" t="s">
+        <v>46</v>
+      </c>
+      <c r="E16" t="s">
         <v>49</v>
       </c>
-      <c r="D16" t="s">
-        <v>47</v>
-      </c>
-      <c r="E16" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A17">
         <v>2</v>
       </c>
       <c r="B17" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="C17" t="s">
+        <v>50</v>
+      </c>
+      <c r="D17" t="s">
         <v>51</v>
       </c>
-      <c r="D17" t="s">
-        <v>52</v>
-      </c>
       <c r="E17" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A18">
         <v>1</v>
       </c>
       <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
         <v>53</v>
       </c>
-      <c r="C18" t="s">
+      <c r="D18" t="s">
         <v>54</v>
       </c>
-      <c r="D18" t="s">
-        <v>55</v>
-      </c>
       <c r="E18" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A19">
         <v>1</v>
       </c>
       <c r="B19" t="s">
+        <v>55</v>
+      </c>
+      <c r="C19" t="s">
         <v>56</v>
       </c>
-      <c r="C19" t="s">
+      <c r="D19" t="s">
         <v>57</v>
       </c>
-      <c r="D19" t="s">
-        <v>58</v>
-      </c>
       <c r="E19" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A20">
         <v>1</v>
       </c>
       <c r="B20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
         <v>59</v>
       </c>
-      <c r="C20" t="s">
+      <c r="D20" t="s">
         <v>60</v>
       </c>
-      <c r="D20" t="s">
+      <c r="E20" t="s">
         <v>61</v>
       </c>
-      <c r="E20" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A21">
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>62</v>
+      </c>
+      <c r="C21" t="s">
         <v>63</v>
       </c>
-      <c r="C21" t="s">
+      <c r="D21" t="s">
         <v>64</v>
       </c>
-      <c r="D21" t="s">
-        <v>65</v>
-      </c>
       <c r="E21" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A22">
         <v>1</v>
       </c>
       <c r="B22" t="s">
+        <v>65</v>
+      </c>
+      <c r="C22" t="s">
         <v>66</v>
       </c>
-      <c r="C22" t="s">
+      <c r="D22" t="s">
         <v>67</v>
       </c>
-      <c r="D22" t="s">
+      <c r="E22" t="s">
         <v>68</v>
       </c>
-      <c r="E22" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A23">
         <v>1</v>
       </c>
       <c r="B23" t="s">
+        <v>69</v>
+      </c>
+      <c r="C23" t="s">
         <v>70</v>
       </c>
-      <c r="C23" t="s">
+      <c r="D23" t="s">
         <v>71</v>
       </c>
-      <c r="D23" t="s">
-        <v>72</v>
-      </c>
       <c r="E23" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>